<commit_message>
Commit after including new fixed effects and running analysis as per potential responses to Maluccio comments
</commit_message>
<xml_diff>
--- a/data/NFHS Lockdown Variable List.xlsx
+++ b/data/NFHS Lockdown Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AC536D-B132-4893-B5FD-24FFF236080D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED22A555-D82F-4E85-9FA2-71C26B52964E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="growth" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="917">
   <si>
     <t>Country Code</t>
   </si>
@@ -2771,6 +2771,12 @@
   </si>
   <si>
     <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Maternal has a job but absent</t>
+  </si>
+  <si>
+    <t>v714a</t>
   </si>
 </sst>
 </file>
@@ -3113,13 +3119,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3863,169 +3869,180 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="4" t="s">
+      <c r="A66" t="s">
+        <v>915</v>
+      </c>
+      <c r="B66" t="s">
+        <v>916</v>
+      </c>
+      <c r="D66" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>54</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>131</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>153</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D68" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>155</v>
-      </c>
-      <c r="B69" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="D69" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="D70" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D71" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B73" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D73" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B76" t="s">
-        <v>139</v>
+        <v>126</v>
+      </c>
+      <c r="D76" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B77" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
-      </c>
-      <c r="D79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D80" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>146</v>
+      </c>
+      <c r="B81" t="s">
+        <v>147</v>
+      </c>
+      <c r="D81" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>148</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>149</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4036,10 +4053,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9300CCAF-57BE-48EF-8DBD-9A646865C50C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -4071,7 +4087,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4088,7 +4104,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4122,7 +4138,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4139,7 +4155,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4190,7 +4206,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4210,7 +4226,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4230,7 +4246,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4247,7 +4263,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4281,7 +4297,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4298,7 +4314,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4332,7 +4348,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4349,7 +4365,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4366,7 +4382,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4400,7 +4416,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4417,7 +4433,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4434,7 +4450,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4451,7 +4467,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4468,7 +4484,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4570,7 +4586,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4604,7 +4620,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4655,7 +4671,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4672,7 +4688,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4689,7 +4705,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4710,13 +4726,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F38" xr:uid="{D2F6BE16-CE6E-482D-A011-873B5C5E0F2F}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Phase 2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F38" xr:uid="{D2F6BE16-CE6E-482D-A011-873B5C5E0F2F}"/>
   <sortState ref="F1:G37">
     <sortCondition ref="G1:G37"/>
   </sortState>

</xml_diff>